<commit_message>
Added images, references + changes to product details and planning
</commit_message>
<xml_diff>
--- a/productDetails.xlsx
+++ b/productDetails.xlsx
@@ -241,20 +241,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="8" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="12">
@@ -740,7 +740,7 @@
   <dimension ref="B1:G16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -760,30 +760,30 @@
       <c r="E1" s="2"/>
     </row>
     <row r="2" spans="2:7" ht="36" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
@@ -818,7 +818,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="10">
+      <c r="B7" s="7">
         <v>1</v>
       </c>
       <c r="C7" s="4" t="str">
@@ -839,7 +839,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="10">
+      <c r="B8" s="7">
         <v>2</v>
       </c>
       <c r="C8" s="4" t="str">
@@ -860,7 +860,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="11">
+      <c r="B9" s="8">
         <v>3</v>
       </c>
       <c r="C9" s="4" t="str">
@@ -881,7 +881,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="11">
+      <c r="B10" s="8">
         <v>4</v>
       </c>
       <c r="C10" s="4" t="str">
@@ -902,7 +902,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="10">
+      <c r="B11" s="7">
         <v>5</v>
       </c>
       <c r="C11" s="4" t="str">
@@ -923,7 +923,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="10">
+      <c r="B12" s="7">
         <v>6</v>
       </c>
       <c r="C12" s="4" t="str">
@@ -944,7 +944,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="11">
+      <c r="B13" s="8">
         <v>7</v>
       </c>
       <c r="C13" s="4" t="str">
@@ -965,7 +965,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="11">
+      <c r="B14" s="8">
         <v>8</v>
       </c>
       <c r="C14" s="4" t="str">
@@ -986,7 +986,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="10">
+      <c r="B15" s="7">
         <v>9</v>
       </c>
       <c r="C15" s="4" t="str">
@@ -1007,7 +1007,7 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="10">
+      <c r="B16" s="7">
         <v>10</v>
       </c>
       <c r="C16" s="4" t="str">

</xml_diff>